<commit_message>
added optional meetings to the log
</commit_message>
<xml_diff>
--- a/Artifacts/Team Meetings - Updated.xlsx
+++ b/Artifacts/Team Meetings - Updated.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cnkeng/Desktop/fall 2020 classes/Software Design/Software-Design-Artifacts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cnkeng/Desktop/fall 2020 classes/Software Design/Software-Design/Artifacts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA17B058-2709-244C-855B-F7D67176870D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27761E9C-02BC-4C43-BC7D-D197A184482A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20660" xr2:uid="{B69BAA51-2B07-4930-841B-9107909D754E}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="TeamF" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">TeamF!$2:$21</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">TeamF!$2:$22</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="66">
   <si>
     <t>Contact Info</t>
   </si>
@@ -179,21 +179,12 @@
     <t>Make sure everyone has access to the Jira board, complete some of the homework as a group, and answer any questions the team may have.</t>
   </si>
   <si>
-    <t>Readdress definition of team roles during class</t>
-  </si>
-  <si>
     <t>Discussed team norms, accessed team project on Jira, and organized team retrospective presentation slide.</t>
   </si>
   <si>
     <t>Have everyone contribute to Jira project to show they have access to the Boards</t>
   </si>
   <si>
-    <t>Everyone agreed to learn Git and also make some edits/comments/issues in the Jira project to show that they have access to it</t>
-  </si>
-  <si>
-    <t>Everyone is going to make a comment or create an issue to show that they have access to the Jira project, if they haven't done so already</t>
-  </si>
-  <si>
     <t>Repeat of yesterday's meeting for those who couldn't attend</t>
   </si>
   <si>
@@ -213,6 +204,36 @@
   </si>
   <si>
     <t>We discussed how everyone's roles will affect the production, planning, and execution of this game, and we also created a timeline for when we should expect certain components to be done.</t>
+  </si>
+  <si>
+    <t>optional/spontaneous meetings</t>
+  </si>
+  <si>
+    <t>30m</t>
+  </si>
+  <si>
+    <t>We tried to fix some GitHub branching issues, and we made it a learning experience regarding pull requests, cloning/forking, and merging.</t>
+  </si>
+  <si>
+    <t>couldn't attend optional/spontaneous meetings</t>
+  </si>
+  <si>
+    <t>We ran into some merging issues and one of the two project configurations (the multiplayer one) is not working for some reason.</t>
+  </si>
+  <si>
+    <t>Readdress definition of team roles during class.</t>
+  </si>
+  <si>
+    <t>Everyone is going to make a comment or create an issue to show that they have access to the Jira project, if they haven't done so already.</t>
+  </si>
+  <si>
+    <t>Michael E is going to try to combine the two tic-tac-toe projects into one.</t>
+  </si>
+  <si>
+    <t>Everyone agreed to learn Git and also make some edits/comments/issues in the Jira project to show that they have access to it.</t>
+  </si>
+  <si>
+    <t>Ever is going to try to combine the two projects into one.</t>
   </si>
 </sst>
 </file>
@@ -289,12 +310,11 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -325,6 +345,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -348,7 +386,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -375,7 +413,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -401,38 +438,63 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -753,104 +815,108 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AV23"/>
+  <dimension ref="A1:AX24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J15" sqref="J15"/>
+      <selection pane="topRight" activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
     <col min="4" max="4" width="25.83203125" customWidth="1"/>
     <col min="5" max="5" width="17.5" customWidth="1"/>
     <col min="6" max="6" width="16.5" customWidth="1"/>
     <col min="7" max="7" width="18.1640625" customWidth="1"/>
     <col min="8" max="8" width="16.6640625" customWidth="1"/>
-    <col min="9" max="9" width="25.1640625" customWidth="1"/>
-    <col min="10" max="18" width="11" customWidth="1"/>
-    <col min="19" max="29" width="12.6640625" customWidth="1"/>
-    <col min="30" max="34" width="12" customWidth="1"/>
+    <col min="9" max="11" width="25.1640625" customWidth="1"/>
+    <col min="12" max="20" width="11" customWidth="1"/>
+    <col min="21" max="31" width="12.6640625" customWidth="1"/>
+    <col min="32" max="36" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E1" s="27" t="s">
+    <row r="1" spans="1:50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E1" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-    </row>
-    <row r="2" spans="1:48" s="24" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="28" t="s">
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+    </row>
+    <row r="2" spans="1:50" s="23" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="23" t="s">
+      <c r="C2" s="38"/>
+      <c r="D2" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="36" t="s">
+      <c r="R2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="36"/>
-      <c r="S2" s="36"/>
-      <c r="T2" s="36"/>
-      <c r="U2" s="36"/>
-      <c r="V2" s="36" t="s">
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
+      <c r="V2" s="39"/>
+      <c r="W2" s="39"/>
+      <c r="X2" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="W2" s="36"/>
-      <c r="X2" s="36"/>
-      <c r="Y2" s="36"/>
-      <c r="Z2" s="36"/>
-      <c r="AA2" s="36"/>
-      <c r="AB2" s="36" t="s">
+      <c r="Y2" s="39"/>
+      <c r="Z2" s="39"/>
+      <c r="AA2" s="39"/>
+      <c r="AB2" s="39"/>
+      <c r="AC2" s="39"/>
+      <c r="AD2" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="AC2" s="36"/>
-      <c r="AD2" s="36"/>
-      <c r="AE2" s="36"/>
-      <c r="AF2" s="36"/>
-      <c r="AG2" s="36"/>
-      <c r="AH2" s="36"/>
-      <c r="AI2" s="36" t="s">
+      <c r="AE2" s="39"/>
+      <c r="AF2" s="39"/>
+      <c r="AG2" s="39"/>
+      <c r="AH2" s="39"/>
+      <c r="AI2" s="39"/>
+      <c r="AJ2" s="39"/>
+      <c r="AK2" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="AJ2" s="36"/>
-      <c r="AK2" s="36"/>
-      <c r="AL2" s="36"/>
-      <c r="AM2" s="36"/>
-      <c r="AN2" s="36"/>
-      <c r="AO2" s="37"/>
-      <c r="AP2" s="37"/>
-      <c r="AQ2" s="37"/>
-      <c r="AR2" s="37"/>
-      <c r="AS2" s="37"/>
-      <c r="AT2" s="23"/>
-      <c r="AU2" s="23"/>
-      <c r="AV2" s="23"/>
-    </row>
-    <row r="3" spans="1:48" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="AL2" s="39"/>
+      <c r="AM2" s="39"/>
+      <c r="AN2" s="39"/>
+      <c r="AO2" s="39"/>
+      <c r="AP2" s="39"/>
+      <c r="AQ2" s="33"/>
+      <c r="AR2" s="33"/>
+      <c r="AS2" s="33"/>
+      <c r="AT2" s="33"/>
+      <c r="AU2" s="33"/>
+      <c r="AV2" s="22"/>
+      <c r="AW2" s="22"/>
+      <c r="AX2" s="22"/>
+    </row>
+    <row r="3" spans="1:50" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="12" t="s">
         <v>6</v>
       </c>
@@ -860,127 +926,133 @@
       <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="34">
+      <c r="D3" s="31">
         <v>44066</v>
       </c>
-      <c r="E3" s="34">
+      <c r="E3" s="31">
         <v>44067</v>
       </c>
-      <c r="F3" s="34">
+      <c r="F3" s="31">
         <v>44068</v>
       </c>
-      <c r="G3" s="34">
+      <c r="G3" s="31">
         <v>44073</v>
       </c>
-      <c r="H3" s="34">
+      <c r="H3" s="31">
         <v>44074</v>
       </c>
-      <c r="I3" s="34">
+      <c r="I3" s="31">
         <v>44075</v>
       </c>
-      <c r="J3" s="34">
+      <c r="J3" s="45">
+        <v>44078</v>
+      </c>
+      <c r="K3" s="45">
+        <v>44079</v>
+      </c>
+      <c r="L3" s="31">
         <v>44080</v>
       </c>
-      <c r="K3" s="34">
+      <c r="M3" s="31">
         <v>44081</v>
       </c>
-      <c r="L3" s="34">
+      <c r="N3" s="31">
         <v>44082</v>
       </c>
-      <c r="M3" s="34">
+      <c r="O3" s="31">
         <v>44087</v>
       </c>
-      <c r="N3" s="34">
+      <c r="P3" s="31">
         <v>44088</v>
       </c>
-      <c r="O3" s="34">
+      <c r="Q3" s="31">
         <v>44089</v>
       </c>
-      <c r="P3" s="34">
+      <c r="R3" s="31">
         <v>44094</v>
       </c>
-      <c r="Q3" s="34">
+      <c r="S3" s="31">
         <v>44095</v>
       </c>
-      <c r="R3" s="34">
+      <c r="T3" s="31">
         <v>44096</v>
       </c>
-      <c r="S3" s="34">
+      <c r="U3" s="31">
         <v>44101</v>
       </c>
-      <c r="T3" s="34">
+      <c r="V3" s="31">
         <v>44102</v>
       </c>
-      <c r="U3" s="34">
+      <c r="W3" s="31">
         <v>44103</v>
       </c>
-      <c r="V3" s="34">
+      <c r="X3" s="31">
         <v>44108</v>
       </c>
-      <c r="W3" s="34">
+      <c r="Y3" s="31">
         <v>44109</v>
       </c>
-      <c r="X3" s="34">
+      <c r="Z3" s="31">
         <v>44110</v>
       </c>
-      <c r="Y3" s="34">
+      <c r="AA3" s="31">
         <v>44115</v>
       </c>
-      <c r="Z3" s="34">
+      <c r="AB3" s="31">
         <v>44116</v>
       </c>
-      <c r="AA3" s="34">
+      <c r="AC3" s="31">
         <v>44117</v>
       </c>
-      <c r="AB3" s="34">
+      <c r="AD3" s="31">
         <v>44122</v>
       </c>
-      <c r="AC3" s="34">
+      <c r="AE3" s="31">
         <v>44123</v>
       </c>
-      <c r="AD3" s="34">
+      <c r="AF3" s="31">
         <v>44124</v>
       </c>
-      <c r="AE3" s="34">
+      <c r="AG3" s="31">
         <v>44129</v>
       </c>
-      <c r="AF3" s="34">
+      <c r="AH3" s="31">
         <v>44130</v>
       </c>
-      <c r="AG3" s="34">
+      <c r="AI3" s="31">
         <v>44131</v>
       </c>
-      <c r="AH3" s="34">
+      <c r="AJ3" s="31">
         <v>44136</v>
       </c>
-      <c r="AI3" s="34">
+      <c r="AK3" s="31">
         <v>44137</v>
       </c>
-      <c r="AJ3" s="34">
+      <c r="AL3" s="31">
         <v>44138</v>
       </c>
-      <c r="AK3" s="34">
+      <c r="AM3" s="31">
         <v>44143</v>
       </c>
-      <c r="AL3" s="35">
+      <c r="AN3" s="32">
         <v>44144</v>
       </c>
-      <c r="AM3" s="35">
+      <c r="AO3" s="32">
         <v>44145</v>
       </c>
-      <c r="AN3" s="34">
+      <c r="AP3" s="31">
         <v>44150</v>
       </c>
-      <c r="AO3" s="38"/>
-      <c r="AP3" s="38"/>
-      <c r="AQ3" s="38"/>
-      <c r="AR3" s="38"/>
-      <c r="AS3" s="38"/>
-      <c r="AT3" s="13"/>
-      <c r="AU3" s="13"/>
+      <c r="AQ3" s="34"/>
+      <c r="AR3" s="34"/>
+      <c r="AS3" s="34"/>
+      <c r="AT3" s="34"/>
+      <c r="AU3" s="34"/>
       <c r="AV3" s="13"/>
-    </row>
-    <row r="4" spans="1:48" ht="13" x14ac:dyDescent="0.15">
+      <c r="AW3" s="13"/>
+      <c r="AX3" s="13"/>
+    </row>
+    <row r="4" spans="1:50" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="11" t="s">
         <v>16</v>
       </c>
@@ -990,52 +1062,58 @@
       <c r="C4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
-      <c r="T4" s="30"/>
-      <c r="U4" s="30"/>
-      <c r="V4" s="30"/>
-      <c r="W4" s="30"/>
-      <c r="X4" s="30"/>
-      <c r="Y4" s="30"/>
-      <c r="Z4" s="30"/>
-      <c r="AA4" s="30"/>
-      <c r="AB4" s="30"/>
-      <c r="AC4" s="30"/>
-      <c r="AD4" s="30"/>
-      <c r="AE4" s="30"/>
-      <c r="AF4" s="30"/>
-      <c r="AG4" s="30"/>
-      <c r="AH4" s="30"/>
-      <c r="AI4" s="31"/>
-    </row>
-    <row r="5" spans="1:48" ht="13" x14ac:dyDescent="0.15">
+      <c r="D4" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="28"/>
+      <c r="R4" s="28"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="28"/>
+      <c r="U4" s="28"/>
+      <c r="V4" s="28"/>
+      <c r="W4" s="28"/>
+      <c r="X4" s="28"/>
+      <c r="Y4" s="28"/>
+      <c r="Z4" s="28"/>
+      <c r="AA4" s="28"/>
+      <c r="AB4" s="28"/>
+      <c r="AC4" s="28"/>
+      <c r="AD4" s="28"/>
+      <c r="AE4" s="28"/>
+      <c r="AF4" s="28"/>
+      <c r="AG4" s="28"/>
+      <c r="AH4" s="28"/>
+      <c r="AI4" s="28"/>
+      <c r="AJ4" s="28"/>
+      <c r="AK4" s="29"/>
+    </row>
+    <row r="5" spans="1:50" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="11" t="s">
         <v>17</v>
       </c>
@@ -1045,50 +1123,52 @@
       <c r="C5" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="32"/>
-      <c r="H5" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="30"/>
-      <c r="O5" s="30"/>
-      <c r="P5" s="30"/>
-      <c r="Q5" s="30"/>
-      <c r="R5" s="30"/>
-      <c r="S5" s="30"/>
-      <c r="T5" s="30"/>
-      <c r="U5" s="30"/>
-      <c r="V5" s="30"/>
-      <c r="W5" s="30"/>
-      <c r="X5" s="30"/>
-      <c r="Y5" s="30"/>
-      <c r="Z5" s="30"/>
-      <c r="AA5" s="30"/>
-      <c r="AB5" s="30"/>
-      <c r="AC5" s="30"/>
-      <c r="AD5" s="30"/>
-      <c r="AE5" s="30"/>
-      <c r="AF5" s="30"/>
-      <c r="AG5" s="30"/>
-      <c r="AH5" s="30"/>
-      <c r="AI5" s="31"/>
-    </row>
-    <row r="6" spans="1:48" ht="13" x14ac:dyDescent="0.15">
+      <c r="D5" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="30"/>
+      <c r="H5" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="28"/>
+      <c r="R5" s="28"/>
+      <c r="S5" s="28"/>
+      <c r="T5" s="28"/>
+      <c r="U5" s="28"/>
+      <c r="V5" s="28"/>
+      <c r="W5" s="28"/>
+      <c r="X5" s="28"/>
+      <c r="Y5" s="28"/>
+      <c r="Z5" s="28"/>
+      <c r="AA5" s="28"/>
+      <c r="AB5" s="28"/>
+      <c r="AC5" s="28"/>
+      <c r="AD5" s="28"/>
+      <c r="AE5" s="28"/>
+      <c r="AF5" s="28"/>
+      <c r="AG5" s="28"/>
+      <c r="AH5" s="28"/>
+      <c r="AI5" s="28"/>
+      <c r="AJ5" s="28"/>
+      <c r="AK5" s="29"/>
+    </row>
+    <row r="6" spans="1:50" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="11" t="s">
         <v>18</v>
       </c>
@@ -1098,48 +1178,52 @@
       <c r="C6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="32"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="30"/>
-      <c r="S6" s="30"/>
-      <c r="T6" s="30"/>
-      <c r="U6" s="30"/>
-      <c r="V6" s="30"/>
-      <c r="W6" s="30"/>
-      <c r="X6" s="30"/>
-      <c r="Y6" s="30"/>
-      <c r="Z6" s="30"/>
-      <c r="AA6" s="30"/>
-      <c r="AB6" s="30"/>
-      <c r="AC6" s="30"/>
-      <c r="AD6" s="30"/>
-      <c r="AE6" s="30"/>
-      <c r="AF6" s="30"/>
-      <c r="AG6" s="30"/>
-      <c r="AH6" s="30"/>
-      <c r="AI6" s="31"/>
-    </row>
-    <row r="7" spans="1:48" ht="13" x14ac:dyDescent="0.15">
+      <c r="D6" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="30"/>
+      <c r="F6" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="30"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="28"/>
+      <c r="R6" s="28"/>
+      <c r="S6" s="28"/>
+      <c r="T6" s="28"/>
+      <c r="U6" s="28"/>
+      <c r="V6" s="28"/>
+      <c r="W6" s="28"/>
+      <c r="X6" s="28"/>
+      <c r="Y6" s="28"/>
+      <c r="Z6" s="28"/>
+      <c r="AA6" s="28"/>
+      <c r="AB6" s="28"/>
+      <c r="AC6" s="28"/>
+      <c r="AD6" s="28"/>
+      <c r="AE6" s="28"/>
+      <c r="AF6" s="28"/>
+      <c r="AG6" s="28"/>
+      <c r="AH6" s="28"/>
+      <c r="AI6" s="28"/>
+      <c r="AJ6" s="28"/>
+      <c r="AK6" s="29"/>
+    </row>
+    <row r="7" spans="1:50" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="11" t="s">
         <v>19</v>
       </c>
@@ -1149,50 +1233,52 @@
       <c r="C7" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="33" t="s">
+      <c r="D7" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="32"/>
-      <c r="H7" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="I7" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="30"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="30"/>
-      <c r="S7" s="30"/>
-      <c r="T7" s="30"/>
-      <c r="U7" s="30"/>
-      <c r="V7" s="30"/>
-      <c r="W7" s="30"/>
-      <c r="X7" s="30"/>
-      <c r="Y7" s="30"/>
-      <c r="Z7" s="30"/>
-      <c r="AA7" s="30"/>
-      <c r="AB7" s="30"/>
-      <c r="AC7" s="30"/>
-      <c r="AD7" s="30"/>
-      <c r="AE7" s="30"/>
-      <c r="AF7" s="30"/>
-      <c r="AG7" s="30"/>
-      <c r="AH7" s="30"/>
-      <c r="AI7" s="31"/>
-    </row>
-    <row r="8" spans="1:48" ht="13" x14ac:dyDescent="0.15">
+      <c r="F7" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="30"/>
+      <c r="H7" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="28"/>
+      <c r="R7" s="28"/>
+      <c r="S7" s="28"/>
+      <c r="T7" s="28"/>
+      <c r="U7" s="28"/>
+      <c r="V7" s="28"/>
+      <c r="W7" s="28"/>
+      <c r="X7" s="28"/>
+      <c r="Y7" s="28"/>
+      <c r="Z7" s="28"/>
+      <c r="AA7" s="28"/>
+      <c r="AB7" s="28"/>
+      <c r="AC7" s="28"/>
+      <c r="AD7" s="28"/>
+      <c r="AE7" s="28"/>
+      <c r="AF7" s="28"/>
+      <c r="AG7" s="28"/>
+      <c r="AH7" s="28"/>
+      <c r="AI7" s="28"/>
+      <c r="AJ7" s="28"/>
+      <c r="AK7" s="29"/>
+    </row>
+    <row r="8" spans="1:50" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="11" t="s">
         <v>21</v>
       </c>
@@ -1202,50 +1288,54 @@
       <c r="C8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="32"/>
-      <c r="I8" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="30"/>
-      <c r="N8" s="30"/>
-      <c r="O8" s="30"/>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="30"/>
-      <c r="R8" s="30"/>
-      <c r="S8" s="30"/>
-      <c r="T8" s="30"/>
-      <c r="U8" s="30"/>
-      <c r="V8" s="30"/>
-      <c r="W8" s="30"/>
-      <c r="X8" s="30"/>
-      <c r="Y8" s="30"/>
-      <c r="Z8" s="30"/>
-      <c r="AA8" s="30"/>
-      <c r="AB8" s="30"/>
-      <c r="AC8" s="30"/>
-      <c r="AD8" s="30"/>
-      <c r="AE8" s="30"/>
-      <c r="AF8" s="30"/>
-      <c r="AG8" s="30"/>
-      <c r="AH8" s="30"/>
-      <c r="AI8" s="31"/>
-    </row>
-    <row r="9" spans="1:48" ht="13" x14ac:dyDescent="0.15">
+      <c r="D8" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="30"/>
+      <c r="I8" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="42"/>
+      <c r="K8" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="28"/>
+      <c r="S8" s="28"/>
+      <c r="T8" s="28"/>
+      <c r="U8" s="28"/>
+      <c r="V8" s="28"/>
+      <c r="W8" s="28"/>
+      <c r="X8" s="28"/>
+      <c r="Y8" s="28"/>
+      <c r="Z8" s="28"/>
+      <c r="AA8" s="28"/>
+      <c r="AB8" s="28"/>
+      <c r="AC8" s="28"/>
+      <c r="AD8" s="28"/>
+      <c r="AE8" s="28"/>
+      <c r="AF8" s="28"/>
+      <c r="AG8" s="28"/>
+      <c r="AH8" s="28"/>
+      <c r="AI8" s="28"/>
+      <c r="AJ8" s="28"/>
+      <c r="AK8" s="29"/>
+    </row>
+    <row r="9" spans="1:50" ht="13" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
         <v>22</v>
       </c>
@@ -1255,50 +1345,56 @@
       <c r="C9" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="32"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="30"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="30"/>
-      <c r="S9" s="30"/>
-      <c r="T9" s="30"/>
-      <c r="U9" s="30"/>
-      <c r="V9" s="30"/>
-      <c r="W9" s="30"/>
-      <c r="X9" s="30"/>
-      <c r="Y9" s="30"/>
-      <c r="Z9" s="30"/>
-      <c r="AA9" s="30"/>
-      <c r="AB9" s="30"/>
-      <c r="AC9" s="30"/>
-      <c r="AD9" s="30"/>
-      <c r="AE9" s="30"/>
-      <c r="AF9" s="30"/>
-      <c r="AG9" s="30"/>
-      <c r="AH9" s="30"/>
-      <c r="AI9" s="31"/>
-    </row>
-    <row r="10" spans="1:48" ht="13" x14ac:dyDescent="0.15">
+      <c r="D9" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="30"/>
+      <c r="J9" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+      <c r="Q9" s="28"/>
+      <c r="R9" s="28"/>
+      <c r="S9" s="28"/>
+      <c r="T9" s="28"/>
+      <c r="U9" s="28"/>
+      <c r="V9" s="28"/>
+      <c r="W9" s="28"/>
+      <c r="X9" s="28"/>
+      <c r="Y9" s="28"/>
+      <c r="Z9" s="28"/>
+      <c r="AA9" s="28"/>
+      <c r="AB9" s="28"/>
+      <c r="AC9" s="28"/>
+      <c r="AD9" s="28"/>
+      <c r="AE9" s="28"/>
+      <c r="AF9" s="28"/>
+      <c r="AG9" s="28"/>
+      <c r="AH9" s="28"/>
+      <c r="AI9" s="28"/>
+      <c r="AJ9" s="28"/>
+      <c r="AK9" s="29"/>
+    </row>
+    <row r="10" spans="1:50" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="11" t="s">
         <v>20</v>
       </c>
@@ -1308,151 +1404,166 @@
       <c r="C10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="33" t="s">
+      <c r="D10" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="33" t="s">
+      <c r="F10" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
-      <c r="O10" s="30"/>
-      <c r="P10" s="30"/>
-      <c r="Q10" s="30"/>
-      <c r="R10" s="30"/>
-      <c r="S10" s="30"/>
-      <c r="T10" s="30"/>
-      <c r="U10" s="30"/>
-      <c r="V10" s="30"/>
-      <c r="W10" s="30"/>
-      <c r="X10" s="30"/>
-      <c r="Y10" s="30"/>
-      <c r="Z10" s="30"/>
-      <c r="AA10" s="30"/>
-      <c r="AB10" s="30"/>
-      <c r="AC10" s="30"/>
-      <c r="AD10" s="30"/>
-      <c r="AE10" s="30"/>
-      <c r="AF10" s="30"/>
-      <c r="AG10" s="30"/>
-      <c r="AH10" s="30"/>
-      <c r="AI10" s="31"/>
-    </row>
-    <row r="11" spans="1:48" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="13" spans="1:48" ht="124" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I10" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="28"/>
+      <c r="S10" s="28"/>
+      <c r="T10" s="28"/>
+      <c r="U10" s="28"/>
+      <c r="V10" s="28"/>
+      <c r="W10" s="28"/>
+      <c r="X10" s="28"/>
+      <c r="Y10" s="28"/>
+      <c r="Z10" s="28"/>
+      <c r="AA10" s="28"/>
+      <c r="AB10" s="28"/>
+      <c r="AC10" s="28"/>
+      <c r="AD10" s="28"/>
+      <c r="AE10" s="28"/>
+      <c r="AF10" s="28"/>
+      <c r="AG10" s="28"/>
+      <c r="AH10" s="28"/>
+      <c r="AI10" s="28"/>
+      <c r="AJ10" s="28"/>
+      <c r="AK10" s="29"/>
+    </row>
+    <row r="11" spans="1:50" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J11" s="40"/>
+      <c r="K11" s="40"/>
+    </row>
+    <row r="13" spans="1:50" ht="124" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="F13" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="G13" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="H13" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="I13" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="19"/>
-      <c r="Q13" s="19"/>
-      <c r="R13" s="19"/>
-      <c r="S13" s="19"/>
-      <c r="T13" s="19"/>
-      <c r="U13" s="19"/>
-      <c r="V13" s="19"/>
-      <c r="W13" s="19"/>
-      <c r="X13" s="19"/>
-      <c r="Y13" s="19"/>
-      <c r="Z13" s="19"/>
-      <c r="AA13" s="19"/>
-      <c r="AB13" s="19"/>
-      <c r="AC13" s="19"/>
-      <c r="AD13" s="19"/>
-      <c r="AE13" s="19"/>
-      <c r="AF13" s="19"/>
-      <c r="AG13" s="19"/>
-      <c r="AH13" s="19"/>
-      <c r="AI13" s="19"/>
-    </row>
-    <row r="14" spans="1:48" s="5" customFormat="1" ht="259" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I13" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="J13" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="K13" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="18"/>
+      <c r="S13" s="18"/>
+      <c r="T13" s="18"/>
+      <c r="U13" s="18"/>
+      <c r="V13" s="18"/>
+      <c r="W13" s="18"/>
+      <c r="X13" s="18"/>
+      <c r="Y13" s="18"/>
+      <c r="Z13" s="18"/>
+      <c r="AA13" s="18"/>
+      <c r="AB13" s="18"/>
+      <c r="AC13" s="18"/>
+      <c r="AD13" s="18"/>
+      <c r="AE13" s="18"/>
+      <c r="AF13" s="18"/>
+      <c r="AG13" s="18"/>
+      <c r="AH13" s="18"/>
+      <c r="AI13" s="18"/>
+      <c r="AJ13" s="18"/>
+      <c r="AK13" s="18"/>
+    </row>
+    <row r="14" spans="1:50" s="5" customFormat="1" ht="259" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="14" t="s">
         <v>39</v>
       </c>
       <c r="C14" s="6"/>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="H14" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="I14" s="20" t="s">
+      <c r="F14" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="I14" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="J14" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="J14"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="20"/>
-      <c r="R14" s="20"/>
-      <c r="S14" s="20"/>
-      <c r="T14" s="20"/>
-      <c r="U14" s="20"/>
-      <c r="V14" s="20"/>
-      <c r="W14" s="20"/>
-      <c r="X14" s="20"/>
-      <c r="Y14" s="20"/>
-      <c r="Z14" s="20"/>
-      <c r="AA14" s="20"/>
-      <c r="AB14" s="20"/>
-      <c r="AC14" s="20"/>
-      <c r="AD14" s="20"/>
-      <c r="AE14" s="20"/>
-      <c r="AF14" s="25"/>
-      <c r="AG14" s="26"/>
-      <c r="AH14" s="20"/>
-      <c r="AI14" s="20"/>
-      <c r="AJ14" s="6"/>
-      <c r="AK14" s="6"/>
+      <c r="K14" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="L14"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="19"/>
+      <c r="T14" s="19"/>
+      <c r="U14" s="19"/>
+      <c r="V14" s="19"/>
+      <c r="W14" s="19"/>
+      <c r="X14" s="19"/>
+      <c r="Y14" s="19"/>
+      <c r="Z14" s="19"/>
+      <c r="AA14" s="19"/>
+      <c r="AB14" s="19"/>
+      <c r="AC14" s="19"/>
+      <c r="AD14" s="19"/>
+      <c r="AE14" s="19"/>
+      <c r="AF14" s="19"/>
+      <c r="AG14" s="19"/>
+      <c r="AH14" s="35"/>
+      <c r="AI14" s="36"/>
+      <c r="AJ14" s="19"/>
+      <c r="AK14" s="19"/>
       <c r="AL14" s="6"/>
       <c r="AM14" s="6"/>
       <c r="AN14" s="6"/>
@@ -1464,58 +1575,64 @@
       <c r="AT14" s="6"/>
       <c r="AU14" s="6"/>
       <c r="AV14" s="6"/>
-    </row>
-    <row r="15" spans="1:48" s="8" customFormat="1" ht="224" x14ac:dyDescent="0.15">
+      <c r="AW14" s="6"/>
+      <c r="AX14" s="6"/>
+    </row>
+    <row r="15" spans="1:50" s="8" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A15" s="14" t="s">
         <v>40</v>
       </c>
       <c r="C15" s="7"/>
-      <c r="D15" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="20" t="s">
+      <c r="D15" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="G15" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="H15" s="20" t="s">
+      <c r="G15" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="H15" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="I15" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="20"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="20"/>
-      <c r="Q15" s="20"/>
-      <c r="R15" s="20"/>
-      <c r="S15" s="20"/>
-      <c r="T15" s="20"/>
-      <c r="U15" s="20"/>
-      <c r="V15" s="20"/>
-      <c r="W15" s="20"/>
-      <c r="X15" s="20"/>
-      <c r="Y15" s="20"/>
-      <c r="Z15" s="20"/>
-      <c r="AA15" s="20"/>
-      <c r="AB15" s="20"/>
-      <c r="AC15" s="20"/>
-      <c r="AD15" s="20"/>
-      <c r="AE15" s="20"/>
-      <c r="AF15" s="20"/>
+      <c r="I15" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="J15" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="K15" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="19"/>
+      <c r="T15" s="19"/>
+      <c r="U15" s="19"/>
+      <c r="V15" s="19"/>
+      <c r="W15" s="19"/>
+      <c r="X15" s="19"/>
+      <c r="Y15" s="19"/>
+      <c r="Z15" s="19"/>
+      <c r="AA15" s="19"/>
+      <c r="AB15" s="19"/>
+      <c r="AC15" s="19"/>
+      <c r="AD15" s="19"/>
+      <c r="AE15" s="19"/>
+      <c r="AF15" s="19"/>
       <c r="AG15" s="19"/>
-      <c r="AH15" s="20"/>
-      <c r="AI15" s="20"/>
-      <c r="AJ15" s="7"/>
-      <c r="AK15" s="7"/>
+      <c r="AH15" s="19"/>
+      <c r="AI15" s="18"/>
+      <c r="AJ15" s="19"/>
+      <c r="AK15" s="19"/>
       <c r="AL15" s="7"/>
       <c r="AM15" s="7"/>
       <c r="AN15" s="7"/>
@@ -1527,94 +1644,113 @@
       <c r="AT15" s="7"/>
       <c r="AU15" s="7"/>
       <c r="AV15" s="7"/>
-    </row>
-    <row r="16" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AW15" s="7"/>
+      <c r="AX15" s="7"/>
+    </row>
+    <row r="16" spans="1:50" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="21">
+      <c r="D16" s="20">
         <v>15</v>
       </c>
-      <c r="E16" s="21">
+      <c r="E16" s="20">
         <v>3</v>
       </c>
-      <c r="F16" s="19">
+      <c r="F16" s="18">
         <v>30</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="18">
         <v>5</v>
       </c>
-      <c r="H16" s="19">
+      <c r="H16" s="18">
         <v>5</v>
       </c>
-      <c r="I16" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="19"/>
-      <c r="O16" s="19"/>
-      <c r="P16" s="19"/>
-      <c r="Q16" s="19"/>
-      <c r="R16" s="19"/>
-      <c r="S16" s="19"/>
-      <c r="T16" s="19"/>
-      <c r="U16" s="19"/>
-      <c r="V16" s="19"/>
-      <c r="W16" s="19"/>
-      <c r="X16" s="19"/>
-      <c r="Y16" s="19"/>
-      <c r="Z16" s="19"/>
-      <c r="AA16" s="19"/>
-      <c r="AB16" s="19"/>
-      <c r="AC16" s="19"/>
-      <c r="AD16" s="19"/>
-      <c r="AE16" s="19"/>
-      <c r="AF16" s="19"/>
-      <c r="AG16" s="19"/>
-      <c r="AH16" s="19"/>
-      <c r="AI16" s="19"/>
-    </row>
-    <row r="17" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I16" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="J16" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="K16" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="18"/>
+      <c r="S16" s="18"/>
+      <c r="T16" s="18"/>
+      <c r="U16" s="18"/>
+      <c r="V16" s="18"/>
+      <c r="W16" s="18"/>
+      <c r="X16" s="18"/>
+      <c r="Y16" s="18"/>
+      <c r="Z16" s="18"/>
+      <c r="AA16" s="18"/>
+      <c r="AB16" s="18"/>
+      <c r="AC16" s="18"/>
+      <c r="AD16" s="18"/>
+      <c r="AE16" s="18"/>
+      <c r="AF16" s="18"/>
+      <c r="AG16" s="18"/>
+      <c r="AH16" s="18"/>
+      <c r="AI16" s="18"/>
+      <c r="AJ16" s="18"/>
+      <c r="AK16" s="18"/>
+    </row>
+    <row r="17" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="B19" s="16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="13" x14ac:dyDescent="0.15">
-      <c r="B20" s="17" t="s">
+    <row r="20" spans="1:21" ht="28" x14ac:dyDescent="0.15">
+      <c r="B20" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="15"/>
+    </row>
+    <row r="21" spans="1:21" ht="13" x14ac:dyDescent="0.15">
+      <c r="B21" s="17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="13" x14ac:dyDescent="0.15">
-      <c r="B21" s="18" t="s">
+    <row r="22" spans="1:21" ht="42" x14ac:dyDescent="0.15">
+      <c r="B22" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="15"/>
-    </row>
-    <row r="23" spans="1:19" ht="13" x14ac:dyDescent="0.15">
-      <c r="S23" s="4"/>
+      <c r="C22" s="15"/>
+    </row>
+    <row r="23" spans="1:21" ht="46" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B23" s="43" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="13" x14ac:dyDescent="0.15">
+      <c r="U24" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="AF14:AG14"/>
+    <mergeCell ref="AK2:AP2"/>
+    <mergeCell ref="AH14:AI14"/>
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:H2"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="P2:U2"/>
-    <mergeCell ref="V2:AA2"/>
-    <mergeCell ref="AB2:AH2"/>
-    <mergeCell ref="AI2:AN2"/>
+    <mergeCell ref="I2:P2"/>
+    <mergeCell ref="R2:W2"/>
+    <mergeCell ref="X2:AC2"/>
+    <mergeCell ref="AD2:AJ2"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
@@ -1628,7 +1764,7 @@
     <brk id="13" max="16383" man="1"/>
   </rowBreaks>
   <colBreaks count="1" manualBreakCount="1">
-    <brk id="30" max="1048575" man="1"/>
+    <brk id="32" max="1048575" man="1"/>
   </colBreaks>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added meeting summary and action items
</commit_message>
<xml_diff>
--- a/Artifacts/Team Meetings - Updated.xlsx
+++ b/Artifacts/Team Meetings - Updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cnkeng/Desktop/fall 2020 classes/Software Design/Software-Design/Artifacts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2035D42B-F4D5-3042-86BB-9A887923849B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD80EAD-630E-2D4D-9715-F14C7EFDA873}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26320" windowHeight="20660" xr2:uid="{B69BAA51-2B07-4930-841B-9107909D754E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20660" xr2:uid="{B69BAA51-2B07-4930-841B-9107909D754E}"/>
   </bookViews>
   <sheets>
     <sheet name="TeamF" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="63">
   <si>
     <t>Contact Info</t>
   </si>
@@ -213,6 +213,18 @@
   </si>
   <si>
     <t>We discussed how everyone's roles will affect the production, planning, and execution of this game, and we also created a timeline for when we should expect certain components to be done.</t>
+  </si>
+  <si>
+    <t>17m</t>
+  </si>
+  <si>
+    <t>Group will come up with bullet points for Team retrospective during tomorrow's meeting. Rob will test the program and report any additionl bugs to the coders.</t>
+  </si>
+  <si>
+    <t>Discuss team Kanban board and what acceptance criteria we need to meet for the issues/tasks in order to mark them as "Done"</t>
+  </si>
+  <si>
+    <t>We went through each of our open issues/bugs and discussed what acceptance critiera was missing in order to declare he item as "Done," we made sure every team member was able to "Pull from Origin" using GitHub desktop to ensure that they had the most up-to-date repo on their system, and we helped our team members open and run the newest game on their computers from the correct branch.</t>
   </si>
 </sst>
 </file>
@@ -348,7 +360,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -392,6 +404,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -755,9 +773,9 @@
   </sheetPr>
   <dimension ref="A1:AV23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K9" sqref="K9"/>
+      <selection pane="topRight" activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -771,81 +789,82 @@
     <col min="7" max="7" width="18.1640625" customWidth="1"/>
     <col min="8" max="8" width="16.6640625" customWidth="1"/>
     <col min="9" max="9" width="25.1640625" customWidth="1"/>
-    <col min="10" max="18" width="11" customWidth="1"/>
+    <col min="10" max="10" width="26.83203125" customWidth="1"/>
+    <col min="11" max="18" width="11" customWidth="1"/>
     <col min="19" max="29" width="12.6640625" customWidth="1"/>
     <col min="30" max="34" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
     </row>
     <row r="2" spans="1:48" s="24" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37" t="s">
+      <c r="C2" s="39"/>
+      <c r="D2" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37" t="s">
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
       <c r="O2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="38" t="s">
+      <c r="P2" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="38"/>
-      <c r="V2" s="38" t="s">
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="40"/>
+      <c r="V2" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="W2" s="38"/>
-      <c r="X2" s="38"/>
-      <c r="Y2" s="38"/>
-      <c r="Z2" s="38"/>
-      <c r="AA2" s="38"/>
-      <c r="AB2" s="38" t="s">
+      <c r="W2" s="40"/>
+      <c r="X2" s="40"/>
+      <c r="Y2" s="40"/>
+      <c r="Z2" s="40"/>
+      <c r="AA2" s="40"/>
+      <c r="AB2" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="AC2" s="38"/>
-      <c r="AD2" s="38"/>
-      <c r="AE2" s="38"/>
-      <c r="AF2" s="38"/>
-      <c r="AG2" s="38"/>
-      <c r="AH2" s="38"/>
-      <c r="AI2" s="38" t="s">
+      <c r="AC2" s="40"/>
+      <c r="AD2" s="40"/>
+      <c r="AE2" s="40"/>
+      <c r="AF2" s="40"/>
+      <c r="AG2" s="40"/>
+      <c r="AH2" s="40"/>
+      <c r="AI2" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="AJ2" s="38"/>
-      <c r="AK2" s="38"/>
-      <c r="AL2" s="38"/>
-      <c r="AM2" s="38"/>
-      <c r="AN2" s="38"/>
-      <c r="AO2" s="32"/>
-      <c r="AP2" s="32"/>
-      <c r="AQ2" s="32"/>
-      <c r="AR2" s="32"/>
-      <c r="AS2" s="32"/>
+      <c r="AJ2" s="40"/>
+      <c r="AK2" s="40"/>
+      <c r="AL2" s="40"/>
+      <c r="AM2" s="40"/>
+      <c r="AN2" s="40"/>
+      <c r="AO2" s="34"/>
+      <c r="AP2" s="34"/>
+      <c r="AQ2" s="34"/>
+      <c r="AR2" s="34"/>
+      <c r="AS2" s="34"/>
       <c r="AT2" s="23"/>
       <c r="AU2" s="23"/>
       <c r="AV2" s="23"/>
@@ -860,122 +879,122 @@
       <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="32">
         <v>44066</v>
       </c>
-      <c r="E3" s="30">
+      <c r="E3" s="32">
         <v>44067</v>
       </c>
-      <c r="F3" s="30">
+      <c r="F3" s="32">
         <v>44068</v>
       </c>
-      <c r="G3" s="30">
+      <c r="G3" s="32">
         <v>44073</v>
       </c>
-      <c r="H3" s="30">
+      <c r="H3" s="32">
         <v>44074</v>
       </c>
-      <c r="I3" s="30">
+      <c r="I3" s="32">
         <v>44075</v>
       </c>
-      <c r="J3" s="30">
+      <c r="J3" s="32">
         <v>44080</v>
       </c>
-      <c r="K3" s="30">
+      <c r="K3" s="32">
         <v>44081</v>
       </c>
-      <c r="L3" s="30">
+      <c r="L3" s="32">
         <v>44082</v>
       </c>
-      <c r="M3" s="30">
+      <c r="M3" s="32">
         <v>44087</v>
       </c>
-      <c r="N3" s="30">
+      <c r="N3" s="32">
         <v>44088</v>
       </c>
-      <c r="O3" s="30">
+      <c r="O3" s="32">
         <v>44089</v>
       </c>
-      <c r="P3" s="30">
+      <c r="P3" s="32">
         <v>44094</v>
       </c>
-      <c r="Q3" s="30">
+      <c r="Q3" s="32">
         <v>44095</v>
       </c>
-      <c r="R3" s="30">
+      <c r="R3" s="32">
         <v>44096</v>
       </c>
-      <c r="S3" s="30">
+      <c r="S3" s="32">
         <v>44101</v>
       </c>
-      <c r="T3" s="30">
+      <c r="T3" s="32">
         <v>44102</v>
       </c>
-      <c r="U3" s="30">
+      <c r="U3" s="32">
         <v>44103</v>
       </c>
-      <c r="V3" s="30">
+      <c r="V3" s="32">
         <v>44108</v>
       </c>
-      <c r="W3" s="30">
+      <c r="W3" s="32">
         <v>44109</v>
       </c>
-      <c r="X3" s="30">
+      <c r="X3" s="32">
         <v>44110</v>
       </c>
-      <c r="Y3" s="30">
+      <c r="Y3" s="32">
         <v>44115</v>
       </c>
-      <c r="Z3" s="30">
+      <c r="Z3" s="32">
         <v>44116</v>
       </c>
-      <c r="AA3" s="30">
+      <c r="AA3" s="32">
         <v>44117</v>
       </c>
-      <c r="AB3" s="30">
+      <c r="AB3" s="32">
         <v>44122</v>
       </c>
-      <c r="AC3" s="30">
+      <c r="AC3" s="32">
         <v>44123</v>
       </c>
-      <c r="AD3" s="30">
+      <c r="AD3" s="32">
         <v>44124</v>
       </c>
-      <c r="AE3" s="30">
+      <c r="AE3" s="32">
         <v>44129</v>
       </c>
-      <c r="AF3" s="30">
+      <c r="AF3" s="32">
         <v>44130</v>
       </c>
-      <c r="AG3" s="30">
+      <c r="AG3" s="32">
         <v>44131</v>
       </c>
-      <c r="AH3" s="30">
+      <c r="AH3" s="32">
         <v>44136</v>
       </c>
-      <c r="AI3" s="30">
+      <c r="AI3" s="32">
         <v>44137</v>
       </c>
-      <c r="AJ3" s="30">
+      <c r="AJ3" s="32">
         <v>44138</v>
       </c>
-      <c r="AK3" s="30">
+      <c r="AK3" s="32">
         <v>44143</v>
       </c>
-      <c r="AL3" s="31">
+      <c r="AL3" s="33">
         <v>44144</v>
       </c>
-      <c r="AM3" s="31">
+      <c r="AM3" s="33">
         <v>44145</v>
       </c>
-      <c r="AN3" s="30">
+      <c r="AN3" s="32">
         <v>44150</v>
       </c>
-      <c r="AO3" s="33"/>
-      <c r="AP3" s="33"/>
-      <c r="AQ3" s="33"/>
-      <c r="AR3" s="33"/>
-      <c r="AS3" s="33"/>
+      <c r="AO3" s="35"/>
+      <c r="AP3" s="35"/>
+      <c r="AQ3" s="35"/>
+      <c r="AR3" s="35"/>
+      <c r="AS3" s="35"/>
       <c r="AT3" s="13"/>
       <c r="AU3" s="13"/>
       <c r="AV3" s="13"/>
@@ -990,52 +1009,52 @@
       <c r="C4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="26"/>
-      <c r="U4" s="26"/>
-      <c r="V4" s="26"/>
-      <c r="W4" s="26"/>
-      <c r="X4" s="26"/>
-      <c r="Y4" s="26"/>
-      <c r="Z4" s="26"/>
-      <c r="AA4" s="26"/>
-      <c r="AB4" s="26"/>
-      <c r="AC4" s="26"/>
-      <c r="AD4" s="26"/>
-      <c r="AE4" s="26"/>
-      <c r="AF4" s="26"/>
-      <c r="AG4" s="26"/>
-      <c r="AH4" s="26"/>
-      <c r="AI4" s="27"/>
+      <c r="D4" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="28"/>
+      <c r="R4" s="28"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="28"/>
+      <c r="U4" s="28"/>
+      <c r="V4" s="28"/>
+      <c r="W4" s="28"/>
+      <c r="X4" s="28"/>
+      <c r="Y4" s="28"/>
+      <c r="Z4" s="28"/>
+      <c r="AA4" s="28"/>
+      <c r="AB4" s="28"/>
+      <c r="AC4" s="28"/>
+      <c r="AD4" s="28"/>
+      <c r="AE4" s="28"/>
+      <c r="AF4" s="28"/>
+      <c r="AG4" s="28"/>
+      <c r="AH4" s="28"/>
+      <c r="AI4" s="29"/>
     </row>
     <row r="5" spans="1:48" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="11" t="s">
@@ -1047,50 +1066,50 @@
       <c r="C5" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="26"/>
-      <c r="R5" s="26"/>
-      <c r="S5" s="26"/>
-      <c r="T5" s="26"/>
-      <c r="U5" s="26"/>
-      <c r="V5" s="26"/>
-      <c r="W5" s="26"/>
-      <c r="X5" s="26"/>
-      <c r="Y5" s="26"/>
-      <c r="Z5" s="26"/>
-      <c r="AA5" s="26"/>
-      <c r="AB5" s="26"/>
-      <c r="AC5" s="26"/>
-      <c r="AD5" s="26"/>
-      <c r="AE5" s="26"/>
-      <c r="AF5" s="26"/>
-      <c r="AG5" s="26"/>
-      <c r="AH5" s="26"/>
-      <c r="AI5" s="27"/>
+      <c r="D5" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="30"/>
+      <c r="H5" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="28"/>
+      <c r="R5" s="28"/>
+      <c r="S5" s="28"/>
+      <c r="T5" s="28"/>
+      <c r="U5" s="28"/>
+      <c r="V5" s="28"/>
+      <c r="W5" s="28"/>
+      <c r="X5" s="28"/>
+      <c r="Y5" s="28"/>
+      <c r="Z5" s="28"/>
+      <c r="AA5" s="28"/>
+      <c r="AB5" s="28"/>
+      <c r="AC5" s="28"/>
+      <c r="AD5" s="28"/>
+      <c r="AE5" s="28"/>
+      <c r="AF5" s="28"/>
+      <c r="AG5" s="28"/>
+      <c r="AH5" s="28"/>
+      <c r="AI5" s="29"/>
     </row>
     <row r="6" spans="1:48" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="11" t="s">
@@ -1102,48 +1121,48 @@
       <c r="C6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="28"/>
-      <c r="F6" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="28"/>
-      <c r="J6" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26"/>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="26"/>
-      <c r="R6" s="26"/>
-      <c r="S6" s="26"/>
-      <c r="T6" s="26"/>
-      <c r="U6" s="26"/>
-      <c r="V6" s="26"/>
-      <c r="W6" s="26"/>
-      <c r="X6" s="26"/>
-      <c r="Y6" s="26"/>
-      <c r="Z6" s="26"/>
-      <c r="AA6" s="26"/>
-      <c r="AB6" s="26"/>
-      <c r="AC6" s="26"/>
-      <c r="AD6" s="26"/>
-      <c r="AE6" s="26"/>
-      <c r="AF6" s="26"/>
-      <c r="AG6" s="26"/>
-      <c r="AH6" s="26"/>
-      <c r="AI6" s="27"/>
+      <c r="D6" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="30"/>
+      <c r="F6" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="30"/>
+      <c r="J6" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="28"/>
+      <c r="R6" s="28"/>
+      <c r="S6" s="28"/>
+      <c r="T6" s="28"/>
+      <c r="U6" s="28"/>
+      <c r="V6" s="28"/>
+      <c r="W6" s="28"/>
+      <c r="X6" s="28"/>
+      <c r="Y6" s="28"/>
+      <c r="Z6" s="28"/>
+      <c r="AA6" s="28"/>
+      <c r="AB6" s="28"/>
+      <c r="AC6" s="28"/>
+      <c r="AD6" s="28"/>
+      <c r="AE6" s="28"/>
+      <c r="AF6" s="28"/>
+      <c r="AG6" s="28"/>
+      <c r="AH6" s="28"/>
+      <c r="AI6" s="29"/>
     </row>
     <row r="7" spans="1:48" ht="13" x14ac:dyDescent="0.15">
       <c r="A7" s="11" t="s">
@@ -1155,50 +1174,50 @@
       <c r="C7" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="29" t="s">
+      <c r="D7" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="28"/>
-      <c r="H7" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="I7" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26"/>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="26"/>
-      <c r="R7" s="26"/>
-      <c r="S7" s="26"/>
-      <c r="T7" s="26"/>
-      <c r="U7" s="26"/>
-      <c r="V7" s="26"/>
-      <c r="W7" s="26"/>
-      <c r="X7" s="26"/>
-      <c r="Y7" s="26"/>
-      <c r="Z7" s="26"/>
-      <c r="AA7" s="26"/>
-      <c r="AB7" s="26"/>
-      <c r="AC7" s="26"/>
-      <c r="AD7" s="26"/>
-      <c r="AE7" s="26"/>
-      <c r="AF7" s="26"/>
-      <c r="AG7" s="26"/>
-      <c r="AH7" s="26"/>
-      <c r="AI7" s="27"/>
+      <c r="F7" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="30"/>
+      <c r="H7" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="28"/>
+      <c r="R7" s="28"/>
+      <c r="S7" s="28"/>
+      <c r="T7" s="28"/>
+      <c r="U7" s="28"/>
+      <c r="V7" s="28"/>
+      <c r="W7" s="28"/>
+      <c r="X7" s="28"/>
+      <c r="Y7" s="28"/>
+      <c r="Z7" s="28"/>
+      <c r="AA7" s="28"/>
+      <c r="AB7" s="28"/>
+      <c r="AC7" s="28"/>
+      <c r="AD7" s="28"/>
+      <c r="AE7" s="28"/>
+      <c r="AF7" s="28"/>
+      <c r="AG7" s="28"/>
+      <c r="AH7" s="28"/>
+      <c r="AI7" s="29"/>
     </row>
     <row r="8" spans="1:48" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="11" t="s">
@@ -1210,48 +1229,48 @@
       <c r="C8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="28"/>
-      <c r="I8" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="28"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
-      <c r="P8" s="26"/>
-      <c r="Q8" s="26"/>
-      <c r="R8" s="26"/>
-      <c r="S8" s="26"/>
-      <c r="T8" s="26"/>
-      <c r="U8" s="26"/>
-      <c r="V8" s="26"/>
-      <c r="W8" s="26"/>
-      <c r="X8" s="26"/>
-      <c r="Y8" s="26"/>
-      <c r="Z8" s="26"/>
-      <c r="AA8" s="26"/>
-      <c r="AB8" s="26"/>
-      <c r="AC8" s="26"/>
-      <c r="AD8" s="26"/>
-      <c r="AE8" s="26"/>
-      <c r="AF8" s="26"/>
-      <c r="AG8" s="26"/>
-      <c r="AH8" s="26"/>
-      <c r="AI8" s="27"/>
+      <c r="D8" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="30"/>
+      <c r="I8" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="30"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="28"/>
+      <c r="S8" s="28"/>
+      <c r="T8" s="28"/>
+      <c r="U8" s="28"/>
+      <c r="V8" s="28"/>
+      <c r="W8" s="28"/>
+      <c r="X8" s="28"/>
+      <c r="Y8" s="28"/>
+      <c r="Z8" s="28"/>
+      <c r="AA8" s="28"/>
+      <c r="AB8" s="28"/>
+      <c r="AC8" s="28"/>
+      <c r="AD8" s="28"/>
+      <c r="AE8" s="28"/>
+      <c r="AF8" s="28"/>
+      <c r="AG8" s="28"/>
+      <c r="AH8" s="28"/>
+      <c r="AI8" s="29"/>
     </row>
     <row r="9" spans="1:48" ht="13" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
@@ -1263,50 +1282,50 @@
       <c r="C9" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="28"/>
-      <c r="J9" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="26"/>
-      <c r="P9" s="26"/>
-      <c r="Q9" s="26"/>
-      <c r="R9" s="26"/>
-      <c r="S9" s="26"/>
-      <c r="T9" s="26"/>
-      <c r="U9" s="26"/>
-      <c r="V9" s="26"/>
-      <c r="W9" s="26"/>
-      <c r="X9" s="26"/>
-      <c r="Y9" s="26"/>
-      <c r="Z9" s="26"/>
-      <c r="AA9" s="26"/>
-      <c r="AB9" s="26"/>
-      <c r="AC9" s="26"/>
-      <c r="AD9" s="26"/>
-      <c r="AE9" s="26"/>
-      <c r="AF9" s="26"/>
-      <c r="AG9" s="26"/>
-      <c r="AH9" s="26"/>
-      <c r="AI9" s="27"/>
+      <c r="D9" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="30"/>
+      <c r="J9" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+      <c r="Q9" s="28"/>
+      <c r="R9" s="28"/>
+      <c r="S9" s="28"/>
+      <c r="T9" s="28"/>
+      <c r="U9" s="28"/>
+      <c r="V9" s="28"/>
+      <c r="W9" s="28"/>
+      <c r="X9" s="28"/>
+      <c r="Y9" s="28"/>
+      <c r="Z9" s="28"/>
+      <c r="AA9" s="28"/>
+      <c r="AB9" s="28"/>
+      <c r="AC9" s="28"/>
+      <c r="AD9" s="28"/>
+      <c r="AE9" s="28"/>
+      <c r="AF9" s="28"/>
+      <c r="AG9" s="28"/>
+      <c r="AH9" s="28"/>
+      <c r="AI9" s="29"/>
     </row>
     <row r="10" spans="1:48" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="11" t="s">
@@ -1318,52 +1337,52 @@
       <c r="C10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="29" t="s">
+      <c r="D10" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="29" t="s">
+      <c r="F10" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="J10" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="26"/>
-      <c r="P10" s="26"/>
-      <c r="Q10" s="26"/>
-      <c r="R10" s="26"/>
-      <c r="S10" s="26"/>
-      <c r="T10" s="26"/>
-      <c r="U10" s="26"/>
-      <c r="V10" s="26"/>
-      <c r="W10" s="26"/>
-      <c r="X10" s="26"/>
-      <c r="Y10" s="26"/>
-      <c r="Z10" s="26"/>
-      <c r="AA10" s="26"/>
-      <c r="AB10" s="26"/>
-      <c r="AC10" s="26"/>
-      <c r="AD10" s="26"/>
-      <c r="AE10" s="26"/>
-      <c r="AF10" s="26"/>
-      <c r="AG10" s="26"/>
-      <c r="AH10" s="26"/>
-      <c r="AI10" s="27"/>
+      <c r="I10" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="28"/>
+      <c r="S10" s="28"/>
+      <c r="T10" s="28"/>
+      <c r="U10" s="28"/>
+      <c r="V10" s="28"/>
+      <c r="W10" s="28"/>
+      <c r="X10" s="28"/>
+      <c r="Y10" s="28"/>
+      <c r="Z10" s="28"/>
+      <c r="AA10" s="28"/>
+      <c r="AB10" s="28"/>
+      <c r="AC10" s="28"/>
+      <c r="AD10" s="28"/>
+      <c r="AE10" s="28"/>
+      <c r="AF10" s="28"/>
+      <c r="AG10" s="28"/>
+      <c r="AH10" s="28"/>
+      <c r="AI10" s="29"/>
     </row>
     <row r="11" spans="1:48" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="13" spans="1:48" ht="124" customHeight="1" x14ac:dyDescent="0.15">
@@ -1387,6 +1406,9 @@
       </c>
       <c r="I13" s="19" t="s">
         <v>54</v>
+      </c>
+      <c r="J13" s="26" t="s">
+        <v>61</v>
       </c>
       <c r="K13" s="19"/>
       <c r="L13" s="19"/>
@@ -1437,7 +1459,9 @@
       <c r="I14" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="J14"/>
+      <c r="J14" s="25" t="s">
+        <v>62</v>
+      </c>
       <c r="K14" s="20"/>
       <c r="L14" s="20"/>
       <c r="M14" s="20"/>
@@ -1459,8 +1483,8 @@
       <c r="AC14" s="20"/>
       <c r="AD14" s="20"/>
       <c r="AE14" s="20"/>
-      <c r="AF14" s="34"/>
-      <c r="AG14" s="35"/>
+      <c r="AF14" s="36"/>
+      <c r="AG14" s="37"/>
       <c r="AH14" s="20"/>
       <c r="AI14" s="20"/>
       <c r="AJ14" s="6"/>
@@ -1477,7 +1501,7 @@
       <c r="AU14" s="6"/>
       <c r="AV14" s="6"/>
     </row>
-    <row r="15" spans="1:48" s="8" customFormat="1" ht="112" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:48" s="8" customFormat="1" ht="210" x14ac:dyDescent="0.15">
       <c r="A15" s="14" t="s">
         <v>40</v>
       </c>
@@ -1500,7 +1524,9 @@
       <c r="I15" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="J15" s="20"/>
+      <c r="J15" s="20" t="s">
+        <v>60</v>
+      </c>
       <c r="K15" s="20"/>
       <c r="L15" s="20"/>
       <c r="M15" s="20"/>
@@ -1562,7 +1588,9 @@
       <c r="I16" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="J16" s="19"/>
+      <c r="J16" s="19" t="s">
+        <v>59</v>
+      </c>
       <c r="K16" s="19"/>
       <c r="L16" s="19"/>
       <c r="M16" s="19"/>

</xml_diff>